<commit_message>
fix missing image in zdemo_excel16
</commit_message>
<xml_diff>
--- a/src/demos/zdemo_excel16.w3mi.data.xlsx
+++ b/src/demos/zdemo_excel16.w3mi.data.xlsx
@@ -15,12 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Image from a file (c:\Program Files\SAP\FrontEnd\SAPgui\wwi\graphics\W_bio.bmp)</t>
   </si>
   <si>
     <t>Image from web repository (SMW0)</t>
+  </si>
+  <si>
+    <t>Mime repository (by default Question mark in standard Web Dynpro WDT_QUIZ)</t>
   </si>
 </sst>
 </file>
@@ -85,7 +88,7 @@
     <xdr:ext cx="1581150" cy="714375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="0800271CCEE91EDC95BF00BB6297E731"/>
+        <xdr:cNvPr id="1" name="0800271CCEE91EDC95F47F8E0D0591D3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -112,13 +115,40 @@
     <xdr:ext cx="790575" cy="1524000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="0800271CCEE91EDC95BF00BB62980731"/>
+        <xdr:cNvPr id="2" name="0800271CCEE91EDC95F47F8E0D05B1D3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1200150" cy="1381125"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="0800271CCEE91EDC95F47F8E0D05D1D3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
@@ -394,7 +424,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="B2:B8"/>
+  <dimension ref="B2:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" zoomScaleSheetLayoutView="100" workbookViewId="0" showGridLines="1" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -415,6 +445,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="1:2">
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup/>

</xml_diff>